<commit_message>
we are now adding in teh correct Project 3 notebook
</commit_message>
<xml_diff>
--- a/GF_EOM-Rubric.xlsx
+++ b/GF_EOM-Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmsou\Documents\mokum.ai\Goldfinger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D65416B-A6F5-4A92-825E-4F500E67A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC7BC2-B2AE-4995-A720-CF06F4CBD834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1330,7 +1330,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>

</xml_diff>

<commit_message>
Added the correct Porject 5 integration (TV) and the Luqra shit for OEM
</commit_message>
<xml_diff>
--- a/GF_EOM-Rubric.xlsx
+++ b/GF_EOM-Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmsou\Documents\mokum.ai\Goldfinger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC7BC2-B2AE-4995-A720-CF06F4CBD834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B76F4D-C47B-4E08-820A-B17CB444ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>EOM Rubric</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>SIGNAPAY</t>
+  </si>
+  <si>
+    <t>Luqra</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -194,6 +197,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1324,13 +1340,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1583,16 +1599,16 @@
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
         <v>0</v>
       </c>
       <c r="F14" s="4"/>
@@ -1603,16 +1619,16 @@
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
         <v>0</v>
       </c>
       <c r="F15" s="4"/>
@@ -1623,16 +1639,16 @@
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11">
         <v>0.5</v>
       </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
         <v>0</v>
       </c>
       <c r="F16" s="4"/>
@@ -1643,16 +1659,16 @@
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
-        <v>0</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
         <v>0</v>
       </c>
       <c r="F17" s="4"/>
@@ -1663,16 +1679,16 @@
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11">
         <v>0.6</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="11">
         <v>35</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="11">
         <f>D18</f>
         <v>35</v>
       </c>
@@ -1684,16 +1700,16 @@
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="11">
         <v>0.6</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="11">
         <v>35</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="11">
         <f>D19-20</f>
         <v>15</v>
       </c>
@@ -1705,16 +1721,16 @@
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="11">
         <v>0.6</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="11">
         <v>35</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="11">
         <f>D20-20</f>
         <v>15</v>
       </c>
@@ -1726,16 +1742,16 @@
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="11">
         <v>0.6</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="11">
         <v>35</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="11">
         <f>D21-20</f>
         <v>15</v>
       </c>
@@ -1747,16 +1763,16 @@
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="6">
-        <v>0</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B22" s="10">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11">
         <v>0.65</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="11">
         <v>35</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="11">
         <f>D22-15</f>
         <v>20</v>
       </c>
@@ -1768,17 +1784,34 @@
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0</v>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19.899999999999999" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="D24" s="11">
+        <v>35</v>
+      </c>
+      <c r="E24" s="13">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>